<commit_message>
Add documents for classification metrics
</commit_message>
<xml_diff>
--- a/docs/source/_static/notes/table_of_metrics.xlsx
+++ b/docs/source/_static/notes/table_of_metrics.xlsx
@@ -7,14 +7,15 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8616"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
+    <sheet name="1.3.0" sheetId="2" r:id="rId1"/>
+    <sheet name="1.2.2" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="176">
   <si>
     <t>Problem</t>
   </si>
@@ -467,6 +468,81 @@
   </si>
   <si>
     <t>Unknown</t>
+  </si>
+  <si>
+    <t>PS</t>
+  </si>
+  <si>
+    <t>Precision Score</t>
+  </si>
+  <si>
+    <t>NPV</t>
+  </si>
+  <si>
+    <t>Negative Predictive Value</t>
+  </si>
+  <si>
+    <t>RS</t>
+  </si>
+  <si>
+    <t>Recall Score</t>
+  </si>
+  <si>
+    <t>AS</t>
+  </si>
+  <si>
+    <t>Accuracy Score</t>
+  </si>
+  <si>
+    <t>F1S</t>
+  </si>
+  <si>
+    <t>F1 Score</t>
+  </si>
+  <si>
+    <t>F2S</t>
+  </si>
+  <si>
+    <t>F2 Score</t>
+  </si>
+  <si>
+    <t>FBS</t>
+  </si>
+  <si>
+    <t>F-Beta Score</t>
+  </si>
+  <si>
+    <t>SS</t>
+  </si>
+  <si>
+    <t>Specificity Score</t>
+  </si>
+  <si>
+    <t>MCC</t>
+  </si>
+  <si>
+    <t>Matthews Correlation Coefficient</t>
+  </si>
+  <si>
+    <t>HL</t>
+  </si>
+  <si>
+    <t>Hamming Loss</t>
+  </si>
+  <si>
+    <t>LS</t>
+  </si>
+  <si>
+    <t>Lift Score</t>
+  </si>
+  <si>
+    <t>Higher is better (Best = 1), Range = [0, 1]</t>
+  </si>
+  <si>
+    <t>Higher is better (Best = 1), Range = [-1, +1]</t>
+  </si>
+  <si>
+    <t>Higher is better (Best = 0), Range = [0, +inf)</t>
   </si>
 </sst>
 </file>
@@ -890,10 +966,880 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E56"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="20.88671875" style="8" customWidth="1"/>
+    <col min="4" max="4" width="45" style="2" customWidth="1"/>
+    <col min="5" max="5" width="54.77734375" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+      <c r="B11" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+      <c r="B17" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
+      <c r="B20" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="1"/>
+      <c r="B23" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="1"/>
+      <c r="B25" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="1"/>
+      <c r="B26" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="1"/>
+      <c r="B27" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="1"/>
+      <c r="B28" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="1"/>
+      <c r="B29" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="1"/>
+      <c r="B30" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A31" s="1"/>
+      <c r="B31" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A32" s="1"/>
+      <c r="B32" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="1"/>
+      <c r="B33" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A34" s="1"/>
+      <c r="B34" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A35" s="1"/>
+      <c r="B35" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A36" s="1"/>
+      <c r="B36" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A37" s="1"/>
+      <c r="B37" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A38" s="1"/>
+      <c r="B38" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A39" s="1"/>
+      <c r="B39" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A40" s="1"/>
+      <c r="B40" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A41" s="1"/>
+      <c r="B41" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B42" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B43" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B44" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="E44" s="1"/>
+    </row>
+    <row r="45" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A45" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B45" s="6">
+        <v>1</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B46" s="6">
+        <v>2</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B47" s="6">
+        <v>3</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B48" s="6">
+        <v>4</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B49" s="8">
+        <v>5</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B50" s="8">
+        <v>6</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B51" s="8">
+        <v>7</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B52" s="8">
+        <v>8</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B53" s="8">
+        <v>9</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B54" s="8">
+        <v>10</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B55" s="8">
+        <v>11</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B56" s="8">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.8" x14ac:dyDescent="0.3"/>

</xml_diff>